<commit_message>
Fix weird court letter address bug
</commit_message>
<xml_diff>
--- a/minerva/backend/apis/instance/client-master-list.xlsx
+++ b/minerva/backend/apis/instance/client-master-list.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -485,52 +485,64 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Building</t>
+          <t>Clifford</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">1 </t>
+          <t xml:space="preserve">Brooks </t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>3607 112th SW St</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
+          <t>6535 150th SW St</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>TC 01</t>
+        </is>
+      </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Lakewood</t>
+          <t>Tacoma</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>98499</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr"/>
+          <t>98439</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>(425) 209-9897</t>
+        </is>
+      </c>
       <c r="I2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Building</t>
+          <t>Donie</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve">3 </t>
+          <t xml:space="preserve">Rogers </t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2220 97th St S Ct</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
+          <t>6535 150th SW St</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>TC 02</t>
+        </is>
+      </c>
       <c r="F3" t="inlineStr">
         <is>
           <t>Tacoma</t>
@@ -538,34 +550,34 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>98444</t>
+          <t>98439</t>
         </is>
       </c>
       <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Alta Apt</t>
-        </is>
-      </c>
+      <c r="I3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Building</t>
+          <t>Leonidas</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t xml:space="preserve">4 </t>
+          <t xml:space="preserve">England </t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>9807 23rd Ave S Ct</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
+          <t>6535 150th SW St</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>TC 22</t>
+        </is>
+      </c>
       <c r="F4" t="inlineStr">
         <is>
           <t>Tacoma</t>
@@ -573,30 +585,38 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>98444</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr"/>
+          <t>98439</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>(206) 591-1074</t>
+        </is>
+      </c>
       <c r="I4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Building</t>
+          <t>Mary</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t xml:space="preserve">5 </t>
+          <t xml:space="preserve">Newton </t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>9910 24th Ave S Ct</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr"/>
+          <t>6535 150th SW St</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>TC 27</t>
+        </is>
+      </c>
       <c r="F5" t="inlineStr">
         <is>
           <t>Tacoma</t>
@@ -604,11 +624,1103 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>98444</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr"/>
+          <t>98439</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>(253) 348-6355</t>
+        </is>
+      </c>
       <c r="I5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Ida</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Parks </t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>6535 150th SW St</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>TC 60</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Tacoma</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>98439</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>(253) 376-9438</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Whitney</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ringseth </t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>6535 150th SW St</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>TC 70</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Tacoma</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>98439</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>(253) 326-1681</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Michael</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wise </t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>6535 150th SW St</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>TC 71</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Tacoma</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>98439</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>(253) 300-8111</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Jamir</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Jackson </t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>6535 150th SW St</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>TC 96</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Tacoma</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>98439</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>(206) 751-5460</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Donghae</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Park </t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>6535 150th SW St</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>TC 120</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Tacoma</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>98439</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>(206) 313-7551</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>David</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sitthideth </t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>6535 150th SW St</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>TC 121</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Tacoma</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>98439</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>(253) 414-2478</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Zach</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Diviney </t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>6535 150th SW St</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>TC 130</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Tacoma</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>98439</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>(253) 754-2848</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>April</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Johnson </t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>6535 150th SW St</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>TC 136</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Tacoma</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>98439</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>(253) 433-1795</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Kelly</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Neubauer </t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>6535 150th SW St</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>TC 141</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Tacoma</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>98439</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>(253) 508-7787</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Theresa</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wilson </t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>6535 150th SW St</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>TC 146</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Tacoma</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>98439</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>(253) 426-9251</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Olga</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Garza </t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>6535 150th SW St</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>TC 151</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Tacoma</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>98439</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>(424) 385-4010</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Devonte</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Webster </t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>6535 150th SW St</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>TC 152</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Tacoma</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>98439</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>(425) 496-5530</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Crystal</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Stapley </t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>6535 150th SW St</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>TC 179</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Tacoma</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>98439</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>(253) 686-8650</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Joseph</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Baskett </t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>6535 150th SW St</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>TC 202</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Tacoma</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>98439</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>(253) 310-2714</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Susan</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ogiba </t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>6535 150th SW St</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>TC 6507</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Tacoma</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>98439</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>(253) 375-9050</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Susan</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Weilenman </t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>6913 150th SW St</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>CE 17</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Lakewood</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>98439</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>(253) 355-3524</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Kim</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hastings </t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>6913 150th SW St</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>CE 18</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Lakewood</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>98439</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>(253) 883-9599</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Rosalin</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wint </t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>6913 150th SW St</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>CE 20</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Lakewood</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>98439</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>(253) 844-6726</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Rene</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Brown </t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>6913 150th SW St</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>CE 21</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Lakewood</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>98439</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>(253) 883-1509</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Janice</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Warren-Lawrence </t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr"/>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>6905 150th SW St</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>CE 23</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Tacoma</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>98439</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>(206) 852-4581</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Karl</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Alexander </t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>6913 150th SW St</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>CE 44</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Lakewood</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>98439</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>(253) 495-8307</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Ed</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Holley </t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>6913 150th SW St</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>CE 52</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Lakewood</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>98439</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>(253) 754-4198</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Sharmaine</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Holliday </t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>6535 150th SW St</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>HP 2B</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Tacoma</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>98439</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>(253) 750-1154</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Raphael</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bropleh </t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr"/>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>6535 150th SW St</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>HP 3A</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Tacoma</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>98439</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>(253) 236-7717</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Joel</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lopez </t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr"/>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>6535 150th SW St</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>HP 4A</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Tacoma</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>98439</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>(253) 359-1953</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Sharon</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">O'Neal </t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr"/>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>6535 150th SW St</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>HP 5C</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Tacoma</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>98439</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>(253) 292-8814</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Zerlina</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr"/>
+      <c r="C32" t="inlineStr"/>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>6535 150th SW St</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>HP 6C</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Tacoma</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>98439</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>(253) 592-9748</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>user</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>ASDFSFF@mailinator.com</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>2327 Court G</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr"/>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Tacoma</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>98405</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>1234567890</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -621,7 +1733,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -684,7 +1796,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>03-27-21</t>
+          <t>05-20-21</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
@@ -698,33 +1810,737 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Building</t>
+          <t>Ida</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve">2 </t>
+          <t>Parks Hospital</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2429 96th S St</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
+          <t>610 Purdue Mall</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Tacoma</t>
+          <t>West Lafayette</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>98444</t>
+          <t>47907</t>
         </is>
       </c>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Ed</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Holley</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>610 Purdue Mall</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>West Lafayette</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>47907</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Karl</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Alexander</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>610 Purdue Mall</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>West Lafayette</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>47907</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Sharon</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>O’Neal</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>610 Purdue Mall</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>5C</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>West Lafayette</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>47907</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Sharmaine</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Holiday</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>610 Purdue Mall</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2B</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>West Lafayette</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>47907</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Kippi</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>King</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>610 Purdue Mall</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>West Lafayette</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>47907</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Kelly</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Neubauer</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>610 Purdue Mall</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>141</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>West Lafayette</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>47907</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Theresa</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Wilson</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>610 Purdue Mall</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>146</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>West Lafayette</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>47907</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Olga</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Garza</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>610 Purdue Mall</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>151</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>West Lafayette</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>47907</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Devonte</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Webster</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>610 Purdue Mall</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>152</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>West Lafayette</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>47907</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Crystal</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Stapley</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>610 Purdue Mall</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>179</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>West Lafayette</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>47907</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Joseph</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Baskett</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>610 Purdue Mall</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>202</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>West Lafayette</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>47907</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Susan</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Ogiba</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>610 Purdue Mall</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>6507</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>West Lafayette</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>47907</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Isaiah</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Session</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>610 Purdue Mall</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>131</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>West Lafayette</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>47907</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Clifford</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Brooks</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>610 Purdue Mall</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>West Lafayette</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>47907</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Leonidas</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>England</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>610 Purdue Mall</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>West Lafayette</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>47907</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Michael</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Wise</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>610 Purdue Mall</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>71</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>West Lafayette</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>47907</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Donghae</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Park</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>610 Purdue Mall</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>West Lafayette</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>47907</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>David</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Sitthideth</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>610 Purdue Mall</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>121</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>West Lafayette</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>47907</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Zach</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Diviney</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>610 Purdue Mall</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>West Lafayette</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>47907</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>April</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Johnson</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>610 Purdue Mall</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>136</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>West Lafayette</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>47907</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr"/>
+      <c r="I23" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>